<commit_message>
updated code to generate and regenerated CPU fig and table
</commit_message>
<xml_diff>
--- a/output_for_paper/table_3.xlsx
+++ b/output_for_paper/table_3.xlsx
@@ -1,61 +1,68 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rozen\Documents\GitHub\mSigHdp_paper_sup_files_x1\output_for_paper\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6A2031-01EB-42DD-AD7D-F9186F3A1C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="51030" yWindow="-8670" windowWidth="13185" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t xml:space="preserve">Approach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBS_set1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBS_set2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average SBS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">indel_set1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">indel_set2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average indel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mSigHdp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mSigHdp_ds_3k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SignatureAnalyzer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">signeR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SigProfilerExtractor</t>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>SBS_set1</t>
+  </si>
+  <si>
+    <t>SBS_set2</t>
+  </si>
+  <si>
+    <t>Average SBS</t>
+  </si>
+  <si>
+    <t>indel_set1</t>
+  </si>
+  <si>
+    <t>indel_set2</t>
+  </si>
+  <si>
+    <t>Average indel</t>
+  </si>
+  <si>
+    <t>mSigHdp_ds_3k</t>
+  </si>
+  <si>
+    <t>mSigHdp</t>
+  </si>
+  <si>
+    <t>SigProfilerExtractor</t>
+  </si>
+  <si>
+    <t>signeR</t>
+  </si>
+  <si>
+    <t>SignatureAnalyzer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -91,6 +98,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -372,14 +388,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,117 +423,114 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="n">
-        <v>205.953724476852</v>
-      </c>
-      <c r="C2" t="n">
-        <v>286.230970212963</v>
-      </c>
-      <c r="D2" t="n">
-        <v>246.092347344907</v>
-      </c>
-      <c r="E2" t="n">
-        <v>3.22527194907407</v>
-      </c>
-      <c r="F2" t="n">
-        <v>6.17506443518518</v>
-      </c>
-      <c r="G2" t="n">
-        <v>3.22527194907407</v>
+      <c r="B2">
+        <v>17.3721260416667</v>
+      </c>
+      <c r="C2">
+        <v>34.820789898148099</v>
+      </c>
+      <c r="D2">
+        <v>26.096457969907402</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="n">
-        <v>17.3721260416667</v>
-      </c>
-      <c r="C3" t="n">
-        <v>34.8207898981481</v>
-      </c>
-      <c r="D3" t="n">
-        <v>26.0964579699074</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
+      <c r="B3">
+        <v>205.95372447685199</v>
+      </c>
+      <c r="C3">
+        <v>286.23097021296297</v>
+      </c>
+      <c r="D3">
+        <v>246.09234734490701</v>
+      </c>
+      <c r="E3">
+        <v>3.2252719490740702</v>
+      </c>
+      <c r="F3">
+        <v>6.1750644351851802</v>
+      </c>
+      <c r="G3">
+        <v>3.2252719490740702</v>
+      </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="n">
-        <v>48.2644204675926</v>
-      </c>
-      <c r="C4" t="n">
-        <v>68.7737221666667</v>
-      </c>
-      <c r="D4" t="n">
-        <v>58.5190713171296</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.452690016203704</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1.61930183796296</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.452690016203704</v>
+      <c r="B4">
+        <v>4.24037824074074</v>
+      </c>
+      <c r="C4">
+        <v>24.337552170138899</v>
+      </c>
+      <c r="D4">
+        <v>14.2889652054398</v>
+      </c>
+      <c r="E4">
+        <v>0.651660509259259</v>
+      </c>
+      <c r="F4">
+        <v>1.4875590046296301</v>
+      </c>
+      <c r="G4">
+        <v>0.651660509259259</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>39.7090664976852</v>
       </c>
-      <c r="C5" t="n">
-        <v>17.5881779074074</v>
-      </c>
-      <c r="D5" t="n">
-        <v>28.6486222025463</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2.08570240046296</v>
-      </c>
-      <c r="F5" t="n">
+      <c r="C5">
+        <v>17.588177907407399</v>
+      </c>
+      <c r="D5">
+        <v>28.648622202546299</v>
+      </c>
+      <c r="E5">
+        <v>2.0857024004629601</v>
+      </c>
+      <c r="F5">
         <v>3.27955544212963</v>
       </c>
-      <c r="G5" t="n">
-        <v>2.08570240046296</v>
+      <c r="G5">
+        <v>2.0857024004629601</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="n">
-        <v>4.24037824074074</v>
-      </c>
-      <c r="C6" t="n">
-        <v>24.3375521701389</v>
-      </c>
-      <c r="D6" t="n">
-        <v>14.2889652054398</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.651660509259259</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1.48755900462963</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.651660509259259</v>
+      <c r="B6">
+        <v>48.264420467592601</v>
+      </c>
+      <c r="C6">
+        <v>68.773722166666701</v>
+      </c>
+      <c r="D6">
+        <v>58.519071317129601</v>
+      </c>
+      <c r="E6">
+        <v>0.45269001620370403</v>
+      </c>
+      <c r="F6">
+        <v>1.61930183796296</v>
+      </c>
+      <c r="G6">
+        <v>0.45269001620370403</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrected error in calculating indel average in table 3
</commit_message>
<xml_diff>
--- a/output_for_paper/table_3.xlsx
+++ b/output_for_paper/table_3.xlsx
@@ -1,61 +1,68 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\non-M\github\mSigHdp_paper_sup_files_x1\output_for_paper\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70964FDC-DCF7-40EF-866D-BBFEF98810FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-38510" yWindow="110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t xml:space="preserve">Approach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBS_set1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBS_set2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average SBS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">indel_set1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">indel_set2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average indel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mSigHdp_ds_3k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mSigHdp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SigProfilerExtractor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">signeR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SignatureAnalyzer</t>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>SBS_set1</t>
+  </si>
+  <si>
+    <t>SBS_set2</t>
+  </si>
+  <si>
+    <t>Average SBS</t>
+  </si>
+  <si>
+    <t>indel_set1</t>
+  </si>
+  <si>
+    <t>indel_set2</t>
+  </si>
+  <si>
+    <t>Average indel</t>
+  </si>
+  <si>
+    <t>mSigHdp_ds_3k</t>
+  </si>
+  <si>
+    <t>mSigHdp</t>
+  </si>
+  <si>
+    <t>SigProfilerExtractor</t>
+  </si>
+  <si>
+    <t>signeR</t>
+  </si>
+  <si>
+    <t>SignatureAnalyzer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -91,6 +98,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -372,14 +388,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,117 +420,114 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="n">
-        <v>15.3125094375</v>
-      </c>
-      <c r="C2" t="n">
-        <v>34.8207898981481</v>
-      </c>
-      <c r="D2" t="n">
-        <v>25.0666496678241</v>
-      </c>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
+      <c r="B2">
+        <v>15.312509437499999</v>
+      </c>
+      <c r="C2">
+        <v>34.820789898148099</v>
+      </c>
+      <c r="D2">
+        <v>25.066649667824102</v>
+      </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="n">
-        <v>205.953724476852</v>
-      </c>
-      <c r="C3" t="n">
-        <v>286.230970212963</v>
-      </c>
-      <c r="D3" t="n">
-        <v>246.092347344907</v>
-      </c>
-      <c r="E3" t="n">
-        <v>3.22527194907407</v>
-      </c>
-      <c r="F3" t="n">
-        <v>6.17506443518518</v>
-      </c>
-      <c r="G3" t="n">
-        <v>3.22527194907407</v>
+      <c r="B3">
+        <v>205.95372447685199</v>
+      </c>
+      <c r="C3">
+        <v>286.23097021296297</v>
+      </c>
+      <c r="D3">
+        <v>246.09234734490701</v>
+      </c>
+      <c r="E3">
+        <v>3.2252719490740702</v>
+      </c>
+      <c r="F3">
+        <v>6.1750644351851802</v>
+      </c>
+      <c r="G3">
+        <v>4.7001681921296301</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>9.15521923611111</v>
       </c>
-      <c r="C4" t="n">
-        <v>24.3365521064815</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4">
+        <v>24.336552106481498</v>
+      </c>
+      <c r="D4">
         <v>16.7458856712963</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>0.651660509259259</v>
       </c>
-      <c r="F4" t="n">
-        <v>1.48755900462963</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.651660509259259</v>
+      <c r="F4">
+        <v>1.4875590046296301</v>
+      </c>
+      <c r="G4">
+        <v>1.06960975694444</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>26.7093536226852</v>
       </c>
-      <c r="C5" t="n">
-        <v>17.5881779074074</v>
-      </c>
-      <c r="D5" t="n">
-        <v>22.1487657650463</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2.08570240046296</v>
-      </c>
-      <c r="F5" t="n">
+      <c r="C5">
+        <v>17.588177907407399</v>
+      </c>
+      <c r="D5">
+        <v>22.148765765046299</v>
+      </c>
+      <c r="E5">
+        <v>2.0857024004629601</v>
+      </c>
+      <c r="F5">
         <v>3.27955544212963</v>
       </c>
-      <c r="G5" t="n">
-        <v>2.08570240046296</v>
+      <c r="G5">
+        <v>2.6826289212962999</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="n">
-        <v>29.1894485902778</v>
-      </c>
-      <c r="C6" t="n">
-        <v>68.7737221666667</v>
-      </c>
-      <c r="D6" t="n">
-        <v>48.9815853784722</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.452690016203704</v>
-      </c>
-      <c r="F6" t="n">
+      <c r="B6">
+        <v>29.189448590277799</v>
+      </c>
+      <c r="C6">
+        <v>68.773722166666701</v>
+      </c>
+      <c r="D6">
+        <v>48.981585378472197</v>
+      </c>
+      <c r="E6">
+        <v>0.45269001620370403</v>
+      </c>
+      <c r="F6">
         <v>1.61930183796296</v>
       </c>
-      <c r="G6" t="n">
-        <v>0.452690016203704</v>
+      <c r="G6">
+        <v>1.0359959270833301</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrected bug in calculating indel average
</commit_message>
<xml_diff>
--- a/output_for_paper/table_3.xlsx
+++ b/output_for_paper/table_3.xlsx
@@ -1,61 +1,68 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\non-M\github\mSigHdp_paper_sup_files_x1\output_for_paper\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70964FDC-DCF7-40EF-866D-BBFEF98810FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-38510" yWindow="110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t xml:space="preserve">Approach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBS_set1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBS_set2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average SBS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">indel_set1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">indel_set2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average indel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mSigHdp_ds_3k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mSigHdp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SigProfilerExtractor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">signeR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SignatureAnalyzer</t>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>SBS_set1</t>
+  </si>
+  <si>
+    <t>SBS_set2</t>
+  </si>
+  <si>
+    <t>Average SBS</t>
+  </si>
+  <si>
+    <t>indel_set1</t>
+  </si>
+  <si>
+    <t>indel_set2</t>
+  </si>
+  <si>
+    <t>Average indel</t>
+  </si>
+  <si>
+    <t>mSigHdp_ds_3k</t>
+  </si>
+  <si>
+    <t>mSigHdp</t>
+  </si>
+  <si>
+    <t>SigProfilerExtractor</t>
+  </si>
+  <si>
+    <t>signeR</t>
+  </si>
+  <si>
+    <t>SignatureAnalyzer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -91,6 +98,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -372,14 +388,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,117 +420,114 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="n">
-        <v>15.3125094375</v>
-      </c>
-      <c r="C2" t="n">
-        <v>34.8207898981481</v>
-      </c>
-      <c r="D2" t="n">
-        <v>25.0666496678241</v>
-      </c>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
+      <c r="B2">
+        <v>15.312509437499999</v>
+      </c>
+      <c r="C2">
+        <v>34.820789898148099</v>
+      </c>
+      <c r="D2">
+        <v>25.066649667824102</v>
+      </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="n">
-        <v>205.953724476852</v>
-      </c>
-      <c r="C3" t="n">
-        <v>286.230970212963</v>
-      </c>
-      <c r="D3" t="n">
-        <v>246.092347344907</v>
-      </c>
-      <c r="E3" t="n">
-        <v>3.22527194907407</v>
-      </c>
-      <c r="F3" t="n">
-        <v>6.17506443518518</v>
-      </c>
-      <c r="G3" t="n">
-        <v>3.22527194907407</v>
+      <c r="B3">
+        <v>205.95372447685199</v>
+      </c>
+      <c r="C3">
+        <v>286.23097021296297</v>
+      </c>
+      <c r="D3">
+        <v>246.09234734490701</v>
+      </c>
+      <c r="E3">
+        <v>3.2252719490740702</v>
+      </c>
+      <c r="F3">
+        <v>6.1750644351851802</v>
+      </c>
+      <c r="G3">
+        <v>4.7001681921296301</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>9.15521923611111</v>
       </c>
-      <c r="C4" t="n">
-        <v>24.3365521064815</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4">
+        <v>24.336552106481498</v>
+      </c>
+      <c r="D4">
         <v>16.7458856712963</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>0.651660509259259</v>
       </c>
-      <c r="F4" t="n">
-        <v>1.48755900462963</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.651660509259259</v>
+      <c r="F4">
+        <v>1.4875590046296301</v>
+      </c>
+      <c r="G4">
+        <v>1.06960975694444</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>26.7093536226852</v>
       </c>
-      <c r="C5" t="n">
-        <v>17.5881779074074</v>
-      </c>
-      <c r="D5" t="n">
-        <v>22.1487657650463</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2.08570240046296</v>
-      </c>
-      <c r="F5" t="n">
+      <c r="C5">
+        <v>17.588177907407399</v>
+      </c>
+      <c r="D5">
+        <v>22.148765765046299</v>
+      </c>
+      <c r="E5">
+        <v>2.0857024004629601</v>
+      </c>
+      <c r="F5">
         <v>3.27955544212963</v>
       </c>
-      <c r="G5" t="n">
-        <v>2.08570240046296</v>
+      <c r="G5">
+        <v>2.6826289212962999</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="n">
-        <v>29.1894485902778</v>
-      </c>
-      <c r="C6" t="n">
-        <v>68.7737221666667</v>
-      </c>
-      <c r="D6" t="n">
-        <v>48.9815853784722</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.452690016203704</v>
-      </c>
-      <c r="F6" t="n">
+      <c r="B6">
+        <v>29.189448590277799</v>
+      </c>
+      <c r="C6">
+        <v>68.773722166666701</v>
+      </c>
+      <c r="D6">
+        <v>48.981585378472197</v>
+      </c>
+      <c r="E6">
+        <v>0.45269001620370403</v>
+      </c>
+      <c r="F6">
         <v>1.61930183796296</v>
       </c>
-      <c r="G6" t="n">
-        <v>0.452690016203704</v>
+      <c r="G6">
+        <v>1.0359959270833301</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>